<commit_message>
Migration + Chon doi vao vong dac biet
</commit_message>
<xml_diff>
--- a/Excel/Giai_Dau2.xlsx
+++ b/Excel/Giai_Dau2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="630" windowWidth="20775" windowHeight="8895"/>
+    <workbookView xWindow="390" yWindow="630" windowWidth="20775" windowHeight="8895" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DS_Giai" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="DS_VDV" sheetId="3" r:id="rId3"/>
     <sheet name="DS_Vong" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="So Do Chọn Doi" sheetId="6" r:id="rId6"/>
+    <sheet name="Bang" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="231">
   <si>
     <t>Ngay</t>
   </si>
@@ -568,12 +570,156 @@
   <si>
     <t>Vòng Bảng</t>
   </si>
+  <si>
+    <t>Số bảng</t>
+  </si>
+  <si>
+    <t>Chọn</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Số cặp tham gia</t>
+  </si>
+  <si>
+    <t>Vòng ĐB</t>
+  </si>
+  <si>
+    <t>Ghi Chú</t>
+  </si>
+  <si>
+    <t>Cặp/Bảng</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Bảng lẻ</t>
+  </si>
+  <si>
+    <t>Tối thiểu</t>
+  </si>
+  <si>
+    <t>Tối đa</t>
+  </si>
+  <si>
+    <t>của 1 cặp</t>
+  </si>
+  <si>
+    <t>Số Bảng</t>
+  </si>
+  <si>
+    <t>1A-2B</t>
+  </si>
+  <si>
+    <t>1B-2A</t>
+  </si>
+  <si>
+    <t>A1-A2</t>
+  </si>
+  <si>
+    <t>A1-B2</t>
+  </si>
+  <si>
+    <t>B1-A2</t>
+  </si>
+  <si>
+    <t>1A-3B/C</t>
+  </si>
+  <si>
+    <t>1B-2C</t>
+  </si>
+  <si>
+    <t>1C-3A/B</t>
+  </si>
+  <si>
+    <t>2A-2B</t>
+  </si>
+  <si>
+    <t>1A-2D</t>
+  </si>
+  <si>
+    <t>1C-2B</t>
+  </si>
+  <si>
+    <t>1D-2A</t>
+  </si>
+  <si>
+    <t>1A-1E</t>
+  </si>
+  <si>
+    <t>1B-2D/C/E/A</t>
+  </si>
+  <si>
+    <t>1C-2A/E/B/D</t>
+  </si>
+  <si>
+    <t>1D-2E/A/B/C</t>
+  </si>
+  <si>
+    <t>1A-2H</t>
+  </si>
+  <si>
+    <t>1B-2G</t>
+  </si>
+  <si>
+    <t>1C-2F</t>
+  </si>
+  <si>
+    <t>1D-2E</t>
+  </si>
+  <si>
+    <t>1E-2D</t>
+  </si>
+  <si>
+    <t>1F-2C</t>
+  </si>
+  <si>
+    <t>1G-2B</t>
+  </si>
+  <si>
+    <t>1H-2A</t>
+  </si>
+  <si>
+    <t>2F-2B</t>
+  </si>
+  <si>
+    <t>2A-2E</t>
+  </si>
+  <si>
+    <t>1C-2D</t>
+  </si>
+  <si>
+    <t>1D-2C</t>
+  </si>
+  <si>
+    <t>1A-3F/E/D/C/B</t>
+  </si>
+  <si>
+    <t>1B-3E/F/D/C/A</t>
+  </si>
+  <si>
+    <t>1F-3A/B/C/D/E</t>
+  </si>
+  <si>
+    <t>1E-3B/A/C/D/F</t>
+  </si>
+  <si>
+    <t>1A-3G/F/E/D/C/B</t>
+  </si>
+  <si>
+    <t>1G-3B/C/D/E/F/G</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -604,13 +750,45 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -625,7 +803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -646,6 +824,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L971" workbookViewId="0">
+    <sheetView topLeftCell="L971" workbookViewId="0">
       <selection activeCell="X1000" sqref="X1000"/>
     </sheetView>
   </sheetViews>
@@ -23693,4 +23895,1584 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="13"/>
+    <col min="7" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" ref="E2:E4" si="0">A2-B2*C2-D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="15">
+        <f>F2*B2+G2+H2</f>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="15">
+        <f t="shared" ref="I3:I63" si="1">F3*B3+G3+H3</f>
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="17">
+        <v>4</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <f>A5-B5*C5-D5</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="17">
+        <v>8</v>
+      </c>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" ref="E6:E63" si="2">A6-B6*C6-D6</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="15">
+        <f t="shared" ref="I11" si="3">F11*B11+G11+H11</f>
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="I17" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="I18" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>7</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="I19" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="I20" s="15">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <v>7</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" s="15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="I22" s="15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="I23" s="15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24" s="15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>26</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="I25" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="I26" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>28</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="I27" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>29</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="I28" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="I29" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="I30" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="I32" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>34</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="I33" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="I34" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>36</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I35" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="I36" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="E37" s="13">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="I37" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>39</v>
+      </c>
+      <c r="E38" s="13">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="I38" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="E39" s="13">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="I39" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="E40" s="13">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="I40" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>42</v>
+      </c>
+      <c r="E41" s="13">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="I41" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>43</v>
+      </c>
+      <c r="E42" s="13">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="I42" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>44</v>
+      </c>
+      <c r="E43" s="13">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="I43" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>45</v>
+      </c>
+      <c r="E44" s="13">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="I44" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>46</v>
+      </c>
+      <c r="E45" s="13">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="I45" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>47</v>
+      </c>
+      <c r="E46" s="13">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="I46" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>48</v>
+      </c>
+      <c r="E47" s="13">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="I47" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>49</v>
+      </c>
+      <c r="E48" s="13">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="I48" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>50</v>
+      </c>
+      <c r="E49" s="13">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="I49" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>51</v>
+      </c>
+      <c r="E50" s="13">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="I50" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>52</v>
+      </c>
+      <c r="E51" s="13">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="I51" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>53</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="I52" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>54</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="I53" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>55</v>
+      </c>
+      <c r="E54" s="13">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="I54" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>56</v>
+      </c>
+      <c r="E55" s="13">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="I55" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>57</v>
+      </c>
+      <c r="E56" s="13">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="I56" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>58</v>
+      </c>
+      <c r="E57" s="13">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="I57" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>59</v>
+      </c>
+      <c r="E58" s="13">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="I58" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>60</v>
+      </c>
+      <c r="E59" s="13">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="I59" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>61</v>
+      </c>
+      <c r="E60" s="13">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="I60" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>62</v>
+      </c>
+      <c r="E61" s="13">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="I61" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>63</v>
+      </c>
+      <c r="E62" s="13">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="I62" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>64</v>
+      </c>
+      <c r="E63" s="13">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="I63" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" style="20" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="20" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="20" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20">
+        <v>2</v>
+      </c>
+      <c r="D1" s="20">
+        <v>3</v>
+      </c>
+      <c r="E1" s="20">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20">
+        <v>5</v>
+      </c>
+      <c r="G1" s="20">
+        <v>6</v>
+      </c>
+      <c r="H1" s="20">
+        <v>7</v>
+      </c>
+      <c r="I1" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="18">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18">
+        <v>4</v>
+      </c>
+      <c r="D2" s="18">
+        <v>8</v>
+      </c>
+      <c r="E2" s="18">
+        <v>8</v>
+      </c>
+      <c r="F2" s="18">
+        <v>8</v>
+      </c>
+      <c r="G2" s="18">
+        <v>16</v>
+      </c>
+      <c r="H2" s="18">
+        <v>16</v>
+      </c>
+      <c r="I2" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G9" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>